<commit_message>
Kod do czujnika ntc110
</commit_message>
<xml_diff>
--- a/iot_warsztaty/czujniki/temp_tabelka.xlsx
+++ b/iot_warsztaty/czujniki/temp_tabelka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jasiu\OneDrive\Dokumenty\!ruzyne takie\Studia\2022PBL Moduły i systemy internetu rzeczy projekt\pbl_repo_hsh\iot_warsztaty\czujniki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9645733-8943-4310-B792-C6B818057CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F40E2B9-076D-4719-A341-B00C1242E682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B9533E36-B50F-40C8-B12D-03841A7B30C8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Czujniki</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>25.50*C~26.60*C</t>
+  </si>
+  <si>
+    <t>PT100</t>
   </si>
 </sst>
 </file>
@@ -460,7 +463,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,8 +514,12 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>

</xml_diff>